<commit_message>
Changed a capacitor part on BOM
</commit_message>
<xml_diff>
--- a/electrical/powersupply/powersupply.xlsx
+++ b/electrical/powersupply/powersupply.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sean\Documents\EECS Capstone Git\eecs-capstone-2122\electrical\powersupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{04F8037E-C9A8-45EA-9679-7D5FF999AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE84220-8735-48F4-B920-E9F145414F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="powersupply" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -256,9 +268,6 @@
     <t>35ZLH100MEFC6.3X11</t>
   </si>
   <si>
-    <t>CL32B106KBJZW6E</t>
-  </si>
-  <si>
     <t>CL10B104KO8NFNC</t>
   </si>
   <si>
@@ -308,12 +317,15 @@
   </si>
   <si>
     <t>TI</t>
+  </si>
+  <si>
+    <t>‎CL32B106KLULNNE‎</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1148,11 +1160,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1259,7 @@
         <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,10 +1279,10 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,10 +1302,10 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,10 +1325,10 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1336,10 +1348,10 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,10 +1371,10 @@
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,10 +1394,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1405,10 +1417,10 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,10 +1440,10 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1485,10 +1497,10 @@
         <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1508,10 +1520,10 @@
         <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1531,10 +1543,10 @@
         <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1554,10 +1566,10 @@
         <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1577,10 +1589,10 @@
         <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1600,10 +1612,10 @@
         <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1623,10 +1635,10 @@
         <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1731,13 +1743,14 @@
         <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>